<commit_message>
Create Autocomplete for Emploees
</commit_message>
<xml_diff>
--- a/docs/Участники проектной работы.xlsx
+++ b/docs/Участники проектной работы.xlsx
@@ -201,10 +201,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -234,10 +243,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -249,8 +259,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1251,8 +1265,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,7 +1377,7 @@
       <c r="C5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1603,26 +1617,29 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1038" r:id="rId4" name="Control 14">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1025" r:id="rId5" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>15</xdr:col>
+                <xdr:col>6</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
+                <xdr:row>0</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>15</xdr:col>
+                <xdr:col>6</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>12</xdr:row>
+                <xdr:row>0</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -1630,24 +1647,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1038" r:id="rId4" name="Control 14"/>
+        <control shapeId="1025" r:id="rId5" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1037" r:id="rId6" name="Control 13">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1026" r:id="rId7" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>6</xdr:col>
+                <xdr:col>15</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
+                <xdr:row>0</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>6</xdr:col>
+                <xdr:col>15</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>12</xdr:row>
+                <xdr:row>0</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -1655,24 +1672,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1037" r:id="rId6" name="Control 13"/>
+        <control shapeId="1026" r:id="rId7" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId7" name="Control 12">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1027" r:id="rId8" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>15</xdr:col>
+                <xdr:col>6</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>15</xdr:col>
+                <xdr:col>6</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>10</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -1680,24 +1697,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1036" r:id="rId7" name="Control 12"/>
+        <control shapeId="1027" r:id="rId8" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId8" name="Control 11">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1028" r:id="rId9" name="Control 4">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>6</xdr:col>
+                <xdr:col>15</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>6</xdr:col>
+                <xdr:col>15</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>10</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -1705,24 +1722,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1035" r:id="rId8" name="Control 11"/>
+        <control shapeId="1028" r:id="rId9" name="Control 4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1034" r:id="rId9" name="Control 10">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1029" r:id="rId10" name="Control 5">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>15</xdr:col>
+                <xdr:col>6</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>15</xdr:col>
+                <xdr:col>6</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>8</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -1730,24 +1747,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1034" r:id="rId9" name="Control 10"/>
+        <control shapeId="1029" r:id="rId10" name="Control 5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId10" name="Control 9">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1030" r:id="rId11" name="Control 6">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>6</xdr:col>
+                <xdr:col>15</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>6</xdr:col>
+                <xdr:col>15</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>8</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -1755,38 +1772,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1033" r:id="rId10" name="Control 9"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId11" name="Control 8">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>15</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>15</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>266700</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1032" r:id="rId11" name="Control 8"/>
+        <control shapeId="1030" r:id="rId11" name="Control 6"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1031" r:id="rId12" name="Control 7">
-          <controlPr defaultSize="0" r:id="rId5">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
@@ -1810,19 +1802,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId13" name="Control 6">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1032" r:id="rId13" name="Control 8">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>15</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>15</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -1830,24 +1822,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1030" r:id="rId13" name="Control 6"/>
+        <control shapeId="1032" r:id="rId13" name="Control 8"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId14" name="Control 5">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1033" r:id="rId14" name="Control 9">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>8</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>8</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -1855,24 +1847,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId14" name="Control 5"/>
+        <control shapeId="1033" r:id="rId14" name="Control 9"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId15" name="Control 4">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1034" r:id="rId15" name="Control 10">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>15</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>8</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>15</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>8</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -1880,24 +1872,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId15" name="Control 4"/>
+        <control shapeId="1034" r:id="rId15" name="Control 10"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId16" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1035" r:id="rId16" name="Control 11">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>10</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>10</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -1905,24 +1897,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId16" name="Control 3"/>
+        <control shapeId="1035" r:id="rId16" name="Control 11"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId17" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1036" r:id="rId17" name="Control 12">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>15</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>0</xdr:row>
+                <xdr:row>10</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>15</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>0</xdr:row>
+                <xdr:row>10</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -1930,24 +1922,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId17" name="Control 2"/>
+        <control shapeId="1036" r:id="rId17" name="Control 12"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId18" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="1037" r:id="rId18" name="Control 13">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>0</xdr:row>
+                <xdr:row>12</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>0</xdr:row>
+                <xdr:row>12</xdr:row>
                 <xdr:rowOff>266700</xdr:rowOff>
               </to>
             </anchor>
@@ -1955,7 +1947,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId18" name="Control 1"/>
+        <control shapeId="1037" r:id="rId18" name="Control 13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1038" r:id="rId19" name="Control 14">
+          <controlPr defaultSize="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>15</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>15</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>266700</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1038" r:id="rId19" name="Control 14"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>